<commit_message>
Auto update (nb+data) - 2025-10-15 17:28:56
</commit_message>
<xml_diff>
--- a/NHL PREDICTIONS.xlsx
+++ b/NHL PREDICTIONS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nic\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0117D0-F0D8-45EA-BA8C-2E8A479FB5D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F77CE006-6F45-4185-BB0D-DCBF999C0A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{24292E02-2EE0-40C4-8B7E-D5191A53C003}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="281">
   <si>
     <t>Random Forest</t>
   </si>
@@ -636,6 +636,249 @@
   </si>
   <si>
     <t>Withdrawal 100$</t>
+  </si>
+  <si>
+    <t>29-01-2025</t>
+  </si>
+  <si>
+    <t>LA vs Panters</t>
+  </si>
+  <si>
+    <t>Floride</t>
+  </si>
+  <si>
+    <t>New jersy</t>
+  </si>
+  <si>
+    <t>Flyer vs New jersey</t>
+  </si>
+  <si>
+    <t>Wild vs Toronto</t>
+  </si>
+  <si>
+    <t>Vancouver vs Nashville</t>
+  </si>
+  <si>
+    <t>Pitt vs Utah</t>
+  </si>
+  <si>
+    <t>Devils vs Flyer</t>
+  </si>
+  <si>
+    <t>Flyers</t>
+  </si>
+  <si>
+    <t>Kings vs Redwing</t>
+  </si>
+  <si>
+    <t>Detroit</t>
+  </si>
+  <si>
+    <t>Canucks vs Blues</t>
+  </si>
+  <si>
+    <t>St louis</t>
+  </si>
+  <si>
+    <t>No bets</t>
+  </si>
+  <si>
+    <t>Kraken vs Oilers</t>
+  </si>
+  <si>
+    <t>Penguins vs Shakrs</t>
+  </si>
+  <si>
+    <t>Penguins</t>
+  </si>
+  <si>
+    <t>27-01-2025</t>
+  </si>
+  <si>
+    <t>Bet Kraken</t>
+  </si>
+  <si>
+    <t>Bet San jose</t>
+  </si>
+  <si>
+    <t>28-01-2025</t>
+  </si>
+  <si>
+    <t>Bos vs buff</t>
+  </si>
+  <si>
+    <t>Buff</t>
+  </si>
+  <si>
+    <t>Winni Montrela</t>
+  </si>
+  <si>
+    <t>Montrea</t>
+  </si>
+  <si>
+    <t>hurricanes vs rangers</t>
+  </si>
+  <si>
+    <t>rangers</t>
+  </si>
+  <si>
+    <t>Black vs Tempa</t>
+  </si>
+  <si>
+    <t>avalanche vs islanders</t>
+  </si>
+  <si>
+    <t>islanders</t>
+  </si>
+  <si>
+    <t>was vs calgary</t>
+  </si>
+  <si>
+    <t>Calgary</t>
+  </si>
+  <si>
+    <t>Ana vs Krak</t>
+  </si>
+  <si>
+    <t>Stars vs Knight</t>
+  </si>
+  <si>
+    <t>Bet black</t>
+  </si>
+  <si>
+    <t>30-1-2025</t>
+  </si>
+  <si>
+    <t>Seattle vs Sharks</t>
+  </si>
+  <si>
+    <t>Knights vs colombus</t>
+  </si>
+  <si>
+    <t>Edmonton vs Red wings</t>
+  </si>
+  <si>
+    <t>Fluers vs Islanders</t>
+  </si>
+  <si>
+    <t>tempa vs LA</t>
+  </si>
+  <si>
+    <t>Ottawa vs Washing</t>
+  </si>
+  <si>
+    <t>Montreal vs Minn</t>
+  </si>
+  <si>
+    <t>Chicago vs Black</t>
+  </si>
+  <si>
+    <t>Bos vs Win</t>
+  </si>
+  <si>
+    <t>31-1-2025</t>
+  </si>
+  <si>
+    <t>Sabres vs Nash</t>
+  </si>
+  <si>
+    <t>Vancouver vs Stars</t>
+  </si>
+  <si>
+    <t>St louis vs Avalanche</t>
+  </si>
+  <si>
+    <t>Colombus vs Utha</t>
+  </si>
+  <si>
+    <t>1-2-2025</t>
+  </si>
+  <si>
+    <t>Black vs Panthers</t>
+  </si>
+  <si>
+    <t>boston</t>
+  </si>
+  <si>
+    <t>Panthers</t>
+  </si>
+  <si>
+    <t>Pits</t>
+  </si>
+  <si>
+    <t>Ptsburg vs Nashville</t>
+  </si>
+  <si>
+    <t>Caro</t>
+  </si>
+  <si>
+    <t>Washing</t>
+  </si>
+  <si>
+    <t>Kings vs Hurrica</t>
+  </si>
+  <si>
+    <t>Islander vs Tempa</t>
+  </si>
+  <si>
+    <t>Jets vs Capitals</t>
+  </si>
+  <si>
+    <t>Wild vs Senators</t>
+  </si>
+  <si>
+    <t>Maple vs Oilers</t>
+  </si>
+  <si>
+    <t>Red Wings vs Flames</t>
+  </si>
+  <si>
+    <t>2-2-2025</t>
+  </si>
+  <si>
+    <t>Devils Sabres</t>
+  </si>
+  <si>
+    <t>Flyer Avalanche</t>
+  </si>
+  <si>
+    <t>Canadiens Duck</t>
+  </si>
+  <si>
+    <t>Islanders Panthers</t>
+  </si>
+  <si>
+    <t>Golden vs Rangers</t>
+  </si>
+  <si>
+    <t>Blue vs stars</t>
+  </si>
+  <si>
+    <t>Blues vs Utah</t>
+  </si>
+  <si>
+    <t>Red wings vs Canucks</t>
+  </si>
+  <si>
+    <t>Flames vs Kraken</t>
+  </si>
+  <si>
+    <t>Bet Flyer</t>
+  </si>
+  <si>
+    <t>Bet Islanders</t>
+  </si>
+  <si>
+    <t>Bet rangers</t>
+  </si>
+  <si>
+    <t>Bet colombus</t>
+  </si>
+  <si>
+    <t>Canuks</t>
+  </si>
+  <si>
+    <t>Bet Calgary</t>
   </si>
 </sst>
 </file>
@@ -1044,10 +1287,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F99FD346-7652-46AB-AEE9-2F50AD839A19}">
-  <dimension ref="A1:L133"/>
+  <dimension ref="A1:L201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="H201" sqref="H201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3602,6 +3845,12 @@
       <c r="E129">
         <v>16.873303571428572</v>
       </c>
+      <c r="F129" t="s">
+        <v>29</v>
+      </c>
+      <c r="G129">
+        <v>0</v>
+      </c>
       <c r="I129" s="1">
         <v>0.5</v>
       </c>
@@ -3625,6 +3874,12 @@
       <c r="E130">
         <v>33.746607142857144</v>
       </c>
+      <c r="F130" t="s">
+        <v>173</v>
+      </c>
+      <c r="G130">
+        <v>58.38</v>
+      </c>
       <c r="I130">
         <v>145.37</v>
       </c>
@@ -3651,6 +3906,16 @@
       <c r="E131">
         <v>6.4897321428571431</v>
       </c>
+      <c r="F131" t="s">
+        <v>173</v>
+      </c>
+      <c r="G131">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="I131">
+        <f>SUM(G129:G133)</f>
+        <v>144.44</v>
+      </c>
       <c r="J131" t="s">
         <v>32</v>
       </c>
@@ -3671,9 +3936,15 @@
       <c r="E132">
         <v>46.72607142857143</v>
       </c>
+      <c r="F132" t="s">
+        <v>29</v>
+      </c>
+      <c r="G132">
+        <v>0</v>
+      </c>
       <c r="I132">
         <f>I131-I130</f>
-        <v>-145.37</v>
+        <v>-0.93000000000000682</v>
       </c>
       <c r="J132" t="s">
         <v>33</v>
@@ -3694,6 +3965,1132 @@
       </c>
       <c r="E133">
         <v>41.534285714285708</v>
+      </c>
+      <c r="F133" t="s">
+        <v>28</v>
+      </c>
+      <c r="G133">
+        <v>76.260000000000005</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>218</v>
+      </c>
+      <c r="B137" t="s">
+        <v>208</v>
+      </c>
+      <c r="C137" t="s">
+        <v>209</v>
+      </c>
+      <c r="E137">
+        <v>25.919999999999998</v>
+      </c>
+      <c r="F137" t="s">
+        <v>28</v>
+      </c>
+      <c r="G137">
+        <v>57.2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>218</v>
+      </c>
+      <c r="B138" t="s">
+        <v>210</v>
+      </c>
+      <c r="C138" t="s">
+        <v>211</v>
+      </c>
+      <c r="E138">
+        <v>28.8</v>
+      </c>
+      <c r="F138" t="s">
+        <v>28</v>
+      </c>
+      <c r="G138">
+        <v>64</v>
+      </c>
+      <c r="J138" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>218</v>
+      </c>
+      <c r="B139" t="s">
+        <v>212</v>
+      </c>
+      <c r="C139" t="s">
+        <v>213</v>
+      </c>
+      <c r="E139" t="s">
+        <v>214</v>
+      </c>
+      <c r="I139">
+        <v>144.44</v>
+      </c>
+      <c r="J139" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>218</v>
+      </c>
+      <c r="B140" t="s">
+        <v>215</v>
+      </c>
+      <c r="C140" t="s">
+        <v>15</v>
+      </c>
+      <c r="E140">
+        <v>15.84</v>
+      </c>
+      <c r="F140" t="s">
+        <v>29</v>
+      </c>
+      <c r="G140">
+        <v>0</v>
+      </c>
+      <c r="I140">
+        <v>212.36</v>
+      </c>
+      <c r="J140" t="s">
+        <v>32</v>
+      </c>
+      <c r="L140" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>218</v>
+      </c>
+      <c r="B141" t="s">
+        <v>216</v>
+      </c>
+      <c r="C141" t="s">
+        <v>217</v>
+      </c>
+      <c r="E141">
+        <v>11.52</v>
+      </c>
+      <c r="F141" t="s">
+        <v>28</v>
+      </c>
+      <c r="G141">
+        <v>28.8</v>
+      </c>
+      <c r="I141">
+        <f>I140-I139</f>
+        <v>67.920000000000016</v>
+      </c>
+      <c r="J141" t="s">
+        <v>33</v>
+      </c>
+      <c r="L141" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E143">
+        <f>SUM(E137:E141)</f>
+        <v>82.08</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>221</v>
+      </c>
+      <c r="B145" t="s">
+        <v>222</v>
+      </c>
+      <c r="C145" t="s">
+        <v>223</v>
+      </c>
+      <c r="D145" s="1">
+        <v>0.64</v>
+      </c>
+      <c r="E145">
+        <v>32.081871345029235</v>
+      </c>
+      <c r="F145" t="s">
+        <v>28</v>
+      </c>
+      <c r="G145">
+        <v>62.47</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>221</v>
+      </c>
+      <c r="B146" t="s">
+        <v>224</v>
+      </c>
+      <c r="C146" t="s">
+        <v>225</v>
+      </c>
+      <c r="D146" s="1">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E146">
+        <v>27.146198830409357</v>
+      </c>
+      <c r="F146" t="s">
+        <v>29</v>
+      </c>
+      <c r="G146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>221</v>
+      </c>
+      <c r="B147" t="s">
+        <v>226</v>
+      </c>
+      <c r="C147" t="s">
+        <v>227</v>
+      </c>
+      <c r="D147" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="E147">
+        <v>17.274853801169591</v>
+      </c>
+      <c r="F147" t="s">
+        <v>29</v>
+      </c>
+      <c r="G147">
+        <v>0</v>
+      </c>
+      <c r="J147" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>221</v>
+      </c>
+      <c r="B148" t="s">
+        <v>228</v>
+      </c>
+      <c r="C148" t="s">
+        <v>43</v>
+      </c>
+      <c r="D148" s="1">
+        <v>0.64</v>
+      </c>
+      <c r="E148">
+        <v>18.508771929824558</v>
+      </c>
+      <c r="F148" t="s">
+        <v>28</v>
+      </c>
+      <c r="G148">
+        <v>45</v>
+      </c>
+      <c r="I148">
+        <v>212.36</v>
+      </c>
+      <c r="J148" t="s">
+        <v>31</v>
+      </c>
+      <c r="L148" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>221</v>
+      </c>
+      <c r="B149" t="s">
+        <v>229</v>
+      </c>
+      <c r="C149" t="s">
+        <v>230</v>
+      </c>
+      <c r="D149" s="1">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E149">
+        <v>28.380116959064328</v>
+      </c>
+      <c r="F149" t="s">
+        <v>28</v>
+      </c>
+      <c r="G149">
+        <v>66</v>
+      </c>
+      <c r="I149">
+        <v>173.47</v>
+      </c>
+      <c r="J149" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>221</v>
+      </c>
+      <c r="B150" t="s">
+        <v>231</v>
+      </c>
+      <c r="C150" t="s">
+        <v>232</v>
+      </c>
+      <c r="D150" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="E150">
+        <v>30.847953216374268</v>
+      </c>
+      <c r="F150" t="s">
+        <v>29</v>
+      </c>
+      <c r="G150">
+        <v>0</v>
+      </c>
+      <c r="I150">
+        <f>I149-I148</f>
+        <v>-38.890000000000015</v>
+      </c>
+      <c r="J150" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>221</v>
+      </c>
+      <c r="B151" t="s">
+        <v>233</v>
+      </c>
+      <c r="C151" t="s">
+        <v>163</v>
+      </c>
+      <c r="D151" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="E151">
+        <v>22.210526315789469</v>
+      </c>
+      <c r="F151" t="s">
+        <v>29</v>
+      </c>
+      <c r="G151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>221</v>
+      </c>
+      <c r="B152" t="s">
+        <v>234</v>
+      </c>
+      <c r="C152" t="s">
+        <v>21</v>
+      </c>
+      <c r="D152" s="1">
+        <v>0.68</v>
+      </c>
+      <c r="E152">
+        <v>34.549707602339183</v>
+      </c>
+      <c r="F152" t="s">
+        <v>29</v>
+      </c>
+      <c r="G152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>200</v>
+      </c>
+      <c r="B156" t="s">
+        <v>201</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D156" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="E156">
+        <v>54.47818181818181</v>
+      </c>
+      <c r="J156" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>200</v>
+      </c>
+      <c r="B157" t="s">
+        <v>204</v>
+      </c>
+      <c r="C157" t="s">
+        <v>203</v>
+      </c>
+      <c r="D157" s="1">
+        <v>0.72</v>
+      </c>
+      <c r="E157">
+        <v>32.973636363636359</v>
+      </c>
+      <c r="I157">
+        <v>173.47</v>
+      </c>
+      <c r="J157" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>200</v>
+      </c>
+      <c r="B158" t="s">
+        <v>205</v>
+      </c>
+      <c r="C158" t="s">
+        <v>18</v>
+      </c>
+      <c r="D158" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="E158">
+        <v>17.20363636363636</v>
+      </c>
+      <c r="J158" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>200</v>
+      </c>
+      <c r="B159" t="s">
+        <v>206</v>
+      </c>
+      <c r="C159" t="s">
+        <v>146</v>
+      </c>
+      <c r="D159" s="1">
+        <v>0.68</v>
+      </c>
+      <c r="E159">
+        <v>30.106363636363632</v>
+      </c>
+      <c r="I159">
+        <f>I158-I157</f>
+        <v>-173.47</v>
+      </c>
+      <c r="J159" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>200</v>
+      </c>
+      <c r="B160" t="s">
+        <v>207</v>
+      </c>
+      <c r="C160" t="s">
+        <v>134</v>
+      </c>
+      <c r="D160" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="E160">
+        <v>38.708181818181814</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E162">
+        <f>SUM(E156:E160)</f>
+        <v>173.46999999999997</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>236</v>
+      </c>
+      <c r="B164" t="s">
+        <v>237</v>
+      </c>
+      <c r="E164">
+        <v>5</v>
+      </c>
+      <c r="F164" t="s">
+        <v>29</v>
+      </c>
+      <c r="G164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>236</v>
+      </c>
+      <c r="B165" t="s">
+        <v>238</v>
+      </c>
+      <c r="E165">
+        <v>6</v>
+      </c>
+      <c r="F165" t="s">
+        <v>28</v>
+      </c>
+      <c r="G165">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>236</v>
+      </c>
+      <c r="B166" t="s">
+        <v>239</v>
+      </c>
+      <c r="E166">
+        <v>13</v>
+      </c>
+      <c r="F166" t="s">
+        <v>28</v>
+      </c>
+      <c r="G166">
+        <v>42.25</v>
+      </c>
+      <c r="J166" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>236</v>
+      </c>
+      <c r="B167" t="s">
+        <v>240</v>
+      </c>
+      <c r="E167">
+        <v>26</v>
+      </c>
+      <c r="F167" t="s">
+        <v>29</v>
+      </c>
+      <c r="G167">
+        <v>0</v>
+      </c>
+      <c r="J167" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>236</v>
+      </c>
+      <c r="B168" t="s">
+        <v>241</v>
+      </c>
+      <c r="E168">
+        <v>19</v>
+      </c>
+      <c r="F168" t="s">
+        <v>28</v>
+      </c>
+      <c r="G168">
+        <v>31.66</v>
+      </c>
+      <c r="J168" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>236</v>
+      </c>
+      <c r="B169" t="s">
+        <v>242</v>
+      </c>
+      <c r="E169">
+        <v>14</v>
+      </c>
+      <c r="F169" t="s">
+        <v>28</v>
+      </c>
+      <c r="G169">
+        <v>26.72</v>
+      </c>
+      <c r="J169" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>236</v>
+      </c>
+      <c r="B170" t="s">
+        <v>243</v>
+      </c>
+      <c r="E170">
+        <v>14</v>
+      </c>
+      <c r="F170" t="s">
+        <v>29</v>
+      </c>
+      <c r="G170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>236</v>
+      </c>
+      <c r="B171" t="s">
+        <v>244</v>
+      </c>
+      <c r="E171">
+        <v>10</v>
+      </c>
+      <c r="F171" t="s">
+        <v>29</v>
+      </c>
+      <c r="G171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>236</v>
+      </c>
+      <c r="B172" t="s">
+        <v>245</v>
+      </c>
+      <c r="E172">
+        <v>30</v>
+      </c>
+      <c r="F172" t="s">
+        <v>29</v>
+      </c>
+      <c r="G172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>246</v>
+      </c>
+      <c r="B175" t="s">
+        <v>247</v>
+      </c>
+      <c r="C175" t="s">
+        <v>151</v>
+      </c>
+      <c r="D175" s="1">
+        <v>0.64</v>
+      </c>
+      <c r="E175">
+        <f>0.3*I177</f>
+        <v>36</v>
+      </c>
+      <c r="F175">
+        <v>73.8</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>246</v>
+      </c>
+      <c r="B176" t="s">
+        <v>248</v>
+      </c>
+      <c r="C176" t="s">
+        <v>20</v>
+      </c>
+      <c r="D176" s="1">
+        <v>0.72</v>
+      </c>
+      <c r="E176">
+        <f>0.24*I177</f>
+        <v>28.799999999999997</v>
+      </c>
+      <c r="F176">
+        <v>46.05</v>
+      </c>
+      <c r="I176" s="1">
+        <v>1</v>
+      </c>
+      <c r="J176" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>246</v>
+      </c>
+      <c r="B177" t="s">
+        <v>249</v>
+      </c>
+      <c r="C177" t="s">
+        <v>17</v>
+      </c>
+      <c r="D177" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="E177">
+        <f>0.13*I177</f>
+        <v>15.600000000000001</v>
+      </c>
+      <c r="F177">
+        <v>24.42</v>
+      </c>
+      <c r="I177">
+        <v>120</v>
+      </c>
+      <c r="J177" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>246</v>
+      </c>
+      <c r="B178" t="s">
+        <v>250</v>
+      </c>
+      <c r="C178" t="s">
+        <v>70</v>
+      </c>
+      <c r="D178" s="1">
+        <v>0.66</v>
+      </c>
+      <c r="E178" t="s">
+        <v>83</v>
+      </c>
+      <c r="I178">
+        <v>183.6</v>
+      </c>
+      <c r="J178" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I179">
+        <f>I178-I177</f>
+        <v>63.599999999999994</v>
+      </c>
+      <c r="J179" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>251</v>
+      </c>
+      <c r="B181" t="s">
+        <v>252</v>
+      </c>
+      <c r="C181" t="s">
+        <v>254</v>
+      </c>
+      <c r="D181" s="1">
+        <v>0.63</v>
+      </c>
+      <c r="E181">
+        <v>23</v>
+      </c>
+      <c r="F181" t="s">
+        <v>29</v>
+      </c>
+      <c r="G181">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>251</v>
+      </c>
+      <c r="B182" t="s">
+        <v>253</v>
+      </c>
+      <c r="C182" t="s">
+        <v>42</v>
+      </c>
+      <c r="D182" s="1">
+        <v>0.64</v>
+      </c>
+      <c r="E182">
+        <v>45</v>
+      </c>
+      <c r="F182" t="s">
+        <v>28</v>
+      </c>
+      <c r="G182">
+        <v>94.5</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>251</v>
+      </c>
+      <c r="B183" t="s">
+        <v>256</v>
+      </c>
+      <c r="C183" t="s">
+        <v>255</v>
+      </c>
+      <c r="D183" s="1">
+        <v>0.64</v>
+      </c>
+      <c r="E183">
+        <f>0.27*I178</f>
+        <v>49.572000000000003</v>
+      </c>
+      <c r="F183" t="s">
+        <v>28</v>
+      </c>
+      <c r="G183">
+        <v>100</v>
+      </c>
+      <c r="I183" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="J183" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>251</v>
+      </c>
+      <c r="B184" t="s">
+        <v>259</v>
+      </c>
+      <c r="C184" t="s">
+        <v>257</v>
+      </c>
+      <c r="D184" s="1">
+        <v>0.69</v>
+      </c>
+      <c r="E184">
+        <f>0.17*I178</f>
+        <v>31.212</v>
+      </c>
+      <c r="F184" t="s">
+        <v>29</v>
+      </c>
+      <c r="G184">
+        <v>0</v>
+      </c>
+      <c r="I184">
+        <v>183.6</v>
+      </c>
+      <c r="J184" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>251</v>
+      </c>
+      <c r="B185" t="s">
+        <v>260</v>
+      </c>
+      <c r="C185" t="s">
+        <v>43</v>
+      </c>
+      <c r="D185" s="1">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E185" t="s">
+        <v>83</v>
+      </c>
+      <c r="I185">
+        <v>178.1</v>
+      </c>
+      <c r="J185" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>251</v>
+      </c>
+      <c r="B186" t="s">
+        <v>261</v>
+      </c>
+      <c r="C186" t="s">
+        <v>258</v>
+      </c>
+      <c r="D186" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="E186" t="s">
+        <v>83</v>
+      </c>
+      <c r="I186">
+        <f>I185-I184</f>
+        <v>-5.5</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>251</v>
+      </c>
+      <c r="B187" t="s">
+        <v>262</v>
+      </c>
+      <c r="C187" t="s">
+        <v>194</v>
+      </c>
+      <c r="D187" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="E187" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>251</v>
+      </c>
+      <c r="B188" t="s">
+        <v>263</v>
+      </c>
+      <c r="C188" t="s">
+        <v>15</v>
+      </c>
+      <c r="D188" s="1">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E188" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>251</v>
+      </c>
+      <c r="B189" t="s">
+        <v>264</v>
+      </c>
+      <c r="C189" t="s">
+        <v>232</v>
+      </c>
+      <c r="D189" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="E189">
+        <f>0.27*I178</f>
+        <v>49.572000000000003</v>
+      </c>
+      <c r="F189" t="s">
+        <v>29</v>
+      </c>
+      <c r="G189">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>265</v>
+      </c>
+      <c r="B193" t="s">
+        <v>266</v>
+      </c>
+      <c r="C193" t="s">
+        <v>151</v>
+      </c>
+      <c r="D193" s="1">
+        <v>0.51</v>
+      </c>
+      <c r="E193">
+        <f>0.1*I197</f>
+        <v>18.36</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>265</v>
+      </c>
+      <c r="B194" t="s">
+        <v>267</v>
+      </c>
+      <c r="C194" t="s">
+        <v>52</v>
+      </c>
+      <c r="D194" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E194">
+        <f>0.14*I197</f>
+        <v>25.704000000000001</v>
+      </c>
+      <c r="H194" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>265</v>
+      </c>
+      <c r="B195" t="s">
+        <v>268</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D195" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="E195">
+        <f>0.07*I197</f>
+        <v>12.852</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>265</v>
+      </c>
+      <c r="B196" t="s">
+        <v>269</v>
+      </c>
+      <c r="C196" t="s">
+        <v>202</v>
+      </c>
+      <c r="D196" s="1">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E196">
+        <f>0.13*I197</f>
+        <v>23.867999999999999</v>
+      </c>
+      <c r="H196" t="s">
+        <v>276</v>
+      </c>
+      <c r="I196" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="J196" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>265</v>
+      </c>
+      <c r="B197" t="s">
+        <v>270</v>
+      </c>
+      <c r="C197" s="1"/>
+      <c r="D197" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E197">
+        <f>0.05*I197</f>
+        <v>9.18</v>
+      </c>
+      <c r="H197" t="s">
+        <v>277</v>
+      </c>
+      <c r="I197">
+        <v>183.6</v>
+      </c>
+      <c r="J197" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>265</v>
+      </c>
+      <c r="B198" t="s">
+        <v>271</v>
+      </c>
+      <c r="C198" t="s">
+        <v>20</v>
+      </c>
+      <c r="D198" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="E198">
+        <f>0.05*I197</f>
+        <v>9.18</v>
+      </c>
+      <c r="H198" t="s">
+        <v>278</v>
+      </c>
+      <c r="J198" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>265</v>
+      </c>
+      <c r="B199" t="s">
+        <v>272</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D199" s="1">
+        <v>0.52</v>
+      </c>
+      <c r="E199" t="s">
+        <v>83</v>
+      </c>
+      <c r="I199">
+        <f>I198-I197</f>
+        <v>-183.6</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>265</v>
+      </c>
+      <c r="B200" t="s">
+        <v>273</v>
+      </c>
+      <c r="C200" t="s">
+        <v>279</v>
+      </c>
+      <c r="D200" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="E200">
+        <f>0.07*I197</f>
+        <v>12.852</v>
+      </c>
+    </row>
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>265</v>
+      </c>
+      <c r="B201" t="s">
+        <v>274</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D201" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="E201">
+        <f>0.04*I197</f>
+        <v>7.3440000000000003</v>
+      </c>
+      <c r="H201" t="s">
+        <v>280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>